<commit_message>
Backlog arrumado, arquivo do python um pouco arrumado, teste de dashboard
</commit_message>
<xml_diff>
--- a/Documentação/Product Backlog.xlsx
+++ b/Documentação/Product Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/joao_hengler_sptech_school/Documents/Sptech/Segundo-Semestre/Pesquisa-E-Inovacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaov\Documents\Repositórios Git\projetobolsa\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{EEC60E2F-90C1-4528-87EE-3B9FB717775E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CA8C976-1CD2-4124-9A0F-EDECC87E052A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1496AD72-E4F8-4570-AF1F-D8B898E1232C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{0B7D7415-480F-42D0-BDD9-2F3E39D055ED}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
   <si>
     <t>Lean Ux Canvas</t>
   </si>
@@ -491,7 +491,7 @@
   <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,6 +742,9 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E22" t="s">

</xml_diff>

<commit_message>
Colocando a modelagem lógica e apagando os arquivos desnecessários do bootstrap
</commit_message>
<xml_diff>
--- a/Documentação/Product Backlog.xlsx
+++ b/Documentação/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaov\Documents\Repositórios Git\projetobolsa\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1496AD72-E4F8-4570-AF1F-D8B898E1232C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD271E7A-2BA8-442E-BA3D-F427AED62DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{0B7D7415-480F-42D0-BDD9-2F3E39D055ED}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>Lean Ux Canvas</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>S1</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13026F67-5EE3-49ED-B266-A9CAAEF4671F}">
-  <dimension ref="B1:F22"/>
+  <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G2" sqref="G2:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,7 +511,7 @@
     <col min="7" max="7" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>15</v>
       </c>
@@ -521,8 +527,11 @@
       <c r="F1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -535,8 +544,11 @@
       <c r="E2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -549,8 +561,11 @@
       <c r="E3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -563,8 +578,11 @@
       <c r="E4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -577,8 +595,11 @@
       <c r="E5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -591,8 +612,11 @@
       <c r="E6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -605,8 +629,11 @@
       <c r="E7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -619,8 +646,11 @@
       <c r="E8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -633,8 +663,11 @@
       <c r="E9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -647,8 +680,11 @@
       <c r="E10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -661,8 +697,11 @@
       <c r="E11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -675,8 +714,11 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -689,8 +731,11 @@
       <c r="E13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -703,8 +748,11 @@
       <c r="E14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>2</v>
       </c>
@@ -717,8 +765,11 @@
       <c r="E15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -731,8 +782,11 @@
       <c r="E16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -745,8 +799,11 @@
       <c r="E17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="E22" t="s">
         <v>19</v>
       </c>

</xml_diff>